<commit_message>
Began to add MessageConfiguration class
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD9B052-891C-47F9-BA2A-7F6DA4AF2648}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A41282E-959E-440E-9730-D2FD4961688A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Issue #</t>
   </si>
@@ -80,13 +80,31 @@
   </si>
   <si>
     <t>Take away '[]' when you have created BroadcastGenerator</t>
+  </si>
+  <si>
+    <t>Citation for MCOS paper here</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>WeightingScheme to be defined</t>
+  </si>
+  <si>
+    <t>config</t>
+  </si>
+  <si>
+    <t>Create a method that can pull out information for a given OMT</t>
+  </si>
+  <si>
+    <t>Build a constructor for MessageConfiguration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +129,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,11 +180,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -442,10 +469,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,21 +482,30 @@
     <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -478,12 +515,8 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -493,27 +526,19 @@
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -524,7 +549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -535,7 +560,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -546,7 +571,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -557,7 +582,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -568,7 +593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -579,32 +604,57 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
config.m before adding PlottingParameters
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A41282E-959E-440E-9730-D2FD4961688A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A14DBBC-745A-4A05-A366-AC5CE5BD58A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Issue #</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Build a constructor for MessageConfiguration</t>
+  </si>
+  <si>
+    <t>Build a conditional statement to set TESLA parameters to null if ECDSA is being used</t>
   </si>
 </sst>
 </file>
@@ -469,11 +472,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +519,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -527,7 +530,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -648,9 +651,440 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Date Created/Completed Fields
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A14DBBC-745A-4A05-A366-AC5CE5BD58A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35350865-60AC-429C-8929-21E889368D0C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Issue #</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>Build a conditional statement to set TESLA parameters to null if ECDSA is being used</t>
+  </si>
+  <si>
+    <t>Date Created</t>
+  </si>
+  <si>
+    <t>Date Completed</t>
   </si>
 </sst>
 </file>
@@ -183,12 +189,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -472,20 +481,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="86.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -495,20 +506,26 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -518,8 +535,11 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="5">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -529,8 +549,14 @@
       <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="6">
+        <v>43542</v>
+      </c>
+      <c r="E3" s="6">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -540,8 +566,14 @@
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="7">
+        <v>43542</v>
+      </c>
+      <c r="E4" s="7">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -551,8 +583,11 @@
       <c r="C5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -562,8 +597,11 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -573,8 +611,11 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -584,8 +625,11 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -595,8 +639,11 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -606,8 +653,11 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -617,8 +667,11 @@
       <c r="C11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -628,8 +681,11 @@
       <c r="C12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -639,8 +695,11 @@
       <c r="C13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -650,8 +709,11 @@
       <c r="C14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -661,8 +723,14 @@
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="7">
+        <v>43542</v>
+      </c>
+      <c r="E15" s="7">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Changed messageConfiguration to OMTConfigurationFile
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CD0215-B601-41A6-A3F4-68395427A9DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCFAD8F-F629-405B-80B9-4D7F3E85B774}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Issue #</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Create a template for creating .mat files for OMTConfiguration using a script in utilities</t>
+  </si>
+  <si>
+    <t>Make key lengths dependent upon the messageConfiguration chosen</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,6 +774,15 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="5">
+        <v>43543</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">

</xml_diff>

<commit_message>
Finished OMTConfigurationGenerator and created ECDSA_RevA.mat
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCFAD8F-F629-405B-80B9-4D7F3E85B774}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA91F27-FE06-4CA2-81D8-FD92FAA5F0AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -497,7 +497,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,21 +756,24 @@
         <v>43543</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="7">
         <v>43543</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="7">
+        <v>43543</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -784,72 +787,72 @@
         <v>43543</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Added sanity check to OMTConfigurationGenerator to avoid future errors
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA91F27-FE06-4CA2-81D8-FD92FAA5F0AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC1DBE6-3523-4A15-AE48-F42B2D741194}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="33">
   <si>
     <t>Issue #</t>
   </si>
@@ -497,7 +497,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,18 +537,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5">
-        <v>43542</v>
+      <c r="D2" s="6">
+        <v>43542</v>
+      </c>
+      <c r="E2" s="6">
+        <v>43543</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1198,6 +1201,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E101">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Moved loadData into utilities directory
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC1DBE6-3523-4A15-AE48-F42B2D741194}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44ADF9C4-DA17-403B-AA75-B9CF0FA67D29}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Issue #</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Make key lengths dependent upon the messageConfiguration chosen</t>
+  </si>
+  <si>
+    <t>Check to make sure that the key lengths in config.m match the loaded OMTConfigurationFile</t>
   </si>
 </sst>
 </file>
@@ -201,7 +204,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -210,6 +213,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -497,7 +501,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +522,7 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -794,6 +798,16 @@
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="5">
+        <v>43543</v>
+      </c>
+      <c r="E19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">

</xml_diff>

<commit_message>
Began making getOTARMessageLengthBits in ConfigParameters
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44ADF9C4-DA17-403B-AA75-B9CF0FA67D29}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34546151-811D-4E7D-8763-0710C328020E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Issue #</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Check to make sure that the key lengths in config.m match the loaded OMTConfigurationFile</t>
+  </si>
+  <si>
+    <t>Create a method for finding how many bits available for OTAR in each authentication frame</t>
   </si>
 </sst>
 </file>
@@ -501,7 +504,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,6 +816,15 @@
       <c r="A20">
         <v>19</v>
       </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="5">
+        <v>43543</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">

</xml_diff>

<commit_message>
Began work on class SBASMessage and subclass SBASAuthenticationMessage
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34546151-811D-4E7D-8763-0710C328020E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502FDDB6-6CF2-4A94-A29B-473890963E7F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="35">
   <si>
     <t>Issue #</t>
   </si>
@@ -504,7 +504,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,16 +813,19 @@
       <c r="E19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="6">
+        <v>43543</v>
+      </c>
+      <c r="E20" s="6">
         <v>43543</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created a class SBASMessage
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502FDDB6-6CF2-4A94-A29B-473890963E7F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572937FF-C25B-423B-8546-B4ECBD37A5F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Issue #</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Create a method for finding how many bits available for OTAR in each authentication frame</t>
+  </si>
+  <si>
+    <t>Grab this information from subclass SBASAuthenticationMessage</t>
+  </si>
+  <si>
+    <t>getOMTFullLength</t>
   </si>
 </sst>
 </file>
@@ -504,7 +510,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,6 +839,15 @@
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="5">
+        <v>43543</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">

</xml_diff>

<commit_message>
Going to start making two different subclasses for each authentication method
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572937FF-C25B-423B-8546-B4ECBD37A5F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAF27B1-B74A-4930-BB94-8437D9A1EE94}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="39">
   <si>
     <t>Issue #</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>getOMTFullLength</t>
+  </si>
+  <si>
+    <t>Make subclasses for SBASECDSAMessage and SBASTESLAMessage</t>
+  </si>
+  <si>
+    <t>SBASMessage</t>
   </si>
 </sst>
 </file>
@@ -510,7 +516,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,6 +859,15 @@
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="5">
+        <v>43543</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">

</xml_diff>

<commit_message>
Finished first pass at OMTConfiguration class
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6356776F-23EE-4AC8-8B3F-0F9E7BD4B9AE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89BE532-95B8-41AE-8C6D-4BCCEB86E169}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,18 +844,21 @@
         <v>43543</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="6">
         <v>43543</v>
+      </c>
+      <c r="E21" s="6">
+        <v>43544</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated OMTConfiguration to read file from configParameters
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89BE532-95B8-41AE-8C6D-4BCCEB86E169}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B098E6-DABD-49EB-844C-1F00546828B5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="40">
   <si>
     <t>Issue #</t>
   </si>
@@ -519,7 +519,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,18 +722,21 @@
         <v>43542</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="5">
-        <v>43542</v>
+      <c r="D13" s="6">
+        <v>43542</v>
+      </c>
+      <c r="E13" s="6">
+        <v>43544</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -767,18 +770,21 @@
         <v>43542</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="7">
         <v>43543</v>
+      </c>
+      <c r="E16" s="7">
+        <v>43544</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Last commit before starting to create OTARSimulator
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7101DA-9AA3-4D74-B3AB-17F927BF22DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D651F11-1E6E-411C-85FE-47D2B797C775}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Issue #</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Delete subclass SBASAuthenticationMessage</t>
+  </si>
+  <si>
+    <t>Make a class for SanityChecks</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,6 +910,16 @@
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="5">
+        <v>43544</v>
+      </c>
+      <c r="E24"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">

</xml_diff>

<commit_message>
Began generating code for broadcast generation and now need to go back and reformat OMTConfiguration
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBD4D54-3279-421A-8AB4-AC603981E84E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E47869-9334-446F-B131-7C52FCB34CBF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Issue #</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>Broadcast</t>
+  </si>
+  <si>
+    <t>Fix OMTConfiguration so the cell locations are related to the message number</t>
+  </si>
+  <si>
+    <t>generateHameedStandardBroadcast</t>
   </si>
 </sst>
 </file>
@@ -534,13 +540,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="86.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
@@ -976,6 +982,15 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="5">
+        <v>43544</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished eVec and sVec in generateHameedStandardBroadcast
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E47869-9334-446F-B131-7C52FCB34CBF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93C1156-84B4-4298-AA0B-AD1C49C9769C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="47">
   <si>
     <t>Issue #</t>
   </si>
@@ -540,7 +540,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,18 +979,21 @@
         <v>43544</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="7">
         <v>43544</v>
+      </c>
+      <c r="E27" s="7">
+        <v>43545</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Broadcast Messages are now generated using generateHameedStandardBroadcast.m!
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93C1156-84B4-4298-AA0B-AD1C49C9769C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA77C357-A2C0-44FA-BD60-1E4D42C043A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Issue #</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>generateHameedStandardBroadcast</t>
+  </si>
+  <si>
+    <t>Write sanity check for the case where PER and weights take on multiple values</t>
+  </si>
+  <si>
+    <t>Make validPERVectorFn</t>
+  </si>
+  <si>
+    <t>Clean up how you do loops!</t>
   </si>
 </sst>
 </file>
@@ -243,7 +252,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -253,6 +262,7 @@
     <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -540,7 +550,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,16 +1010,44 @@
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="5">
+        <v>43545</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="5">
+        <v>43545</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
+      <c r="B30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="9">
+        <v>43545</v>
+      </c>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">

</xml_diff>

<commit_message>
Finished partitionBroadcast, about to start simulateBroadcast
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA77C357-A2C0-44FA-BD60-1E4D42C043A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E0CFEA-B835-4FF0-B7FA-D3F8B6C53F85}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>Issue #</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>Clean up how you do loops!</t>
+  </si>
+  <si>
+    <t>write simulateBroadcast</t>
   </si>
 </sst>
 </file>
@@ -550,7 +553,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,18 +782,21 @@
         <v>43544</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="5">
-        <v>43542</v>
+      <c r="D14" s="7">
+        <v>43542</v>
+      </c>
+      <c r="E14" s="7">
+        <v>43544</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -961,32 +967,38 @@
       </c>
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="7">
         <v>43544</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="E25" s="7">
+        <v>43545</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="7">
         <v>43544</v>
+      </c>
+      <c r="E26" s="7">
+        <v>43545</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1052,6 +1064,15 @@
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="5">
+        <v>43545</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Began to write processBroadcastResults
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E0CFEA-B835-4FF0-B7FA-D3F8B6C53F85}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9886BB69-231A-415F-B7BD-CDC524B69697}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,7 +553,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,17 +1061,20 @@
       </c>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="7">
+        <v>43545</v>
+      </c>
+      <c r="E31" s="7">
         <v>43545</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added getTotalNumUsers to processBroadcastResults
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9886BB69-231A-415F-B7BD-CDC524B69697}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BA184E-1987-44A8-AA63-79FB84F189B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>Issue #</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>write simulateBroadcast</t>
+  </si>
+  <si>
+    <t>Preallocate timeResults</t>
+  </si>
+  <si>
+    <t>processBroadcastResults</t>
   </si>
 </sst>
 </file>
@@ -1082,6 +1088,15 @@
       <c r="A32">
         <v>31</v>
       </c>
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="5">
+        <v>43545</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">

</xml_diff>

<commit_message>
Added plotOTARResults and the code now gives the user the ability to loop through any double variable
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BA184E-1987-44A8-AA63-79FB84F189B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FF88AE-46D5-4921-8F35-58394951CBED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>Issue #</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>processBroadcastResults</t>
+  </si>
+  <si>
+    <t>Make obj = fun(obj) into [] = fun(obj) like calculateObservationData.m</t>
+  </si>
+  <si>
+    <t>Incorporate broadcastGenerator from config.m</t>
   </si>
 </sst>
 </file>
@@ -559,7 +565,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,82 +1104,100 @@
         <v>43545</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="5">
+        <v>43546</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="5">
+        <v>43546</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
About to generalize how OTARSimulation iterations are handled. Wish me luck
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FF88AE-46D5-4921-8F35-58394951CBED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC9DDC3-93A1-4BA7-9B6B-F9C99992EF4C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>Issue #</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Incorporate broadcastGenerator from config.m</t>
+  </si>
+  <si>
+    <t>Make ConfigParameters not a handle and change how iterations are done in OTARSimulator</t>
   </si>
 </sst>
 </file>
@@ -564,8 +567,8 @@
   <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,6 +1139,15 @@
       <c r="A35">
         <v>34</v>
       </c>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="5">
+        <v>43546</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">

</xml_diff>

<commit_message>
Generalized the code base to perform all kinds of sensitivity analyses
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC9DDC3-93A1-4BA7-9B6B-F9C99992EF4C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58440E6A-51A6-4C4F-99D5-E717DB131DD1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Issue #</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Make ConfigParameters not a handle and change how iterations are done in OTARSimulator</t>
+  </si>
+  <si>
+    <t>Change all places where weights are grabbed from omtConfiguration</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,19 +1050,20 @@
         <v>43545</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="6">
         <v>43545</v>
       </c>
+      <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -1152,6 +1156,15 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="5">
+        <v>43546</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First real working version of the new mcos simulator
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58440E6A-51A6-4C4F-99D5-E717DB131DD1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4083A6-089D-4EB8-962F-D0D6DB60E178}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>Issue #</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>Change all places where weights are grabbed from omtConfiguration</t>
+  </si>
+  <si>
+    <t>add plotType to config.m</t>
+  </si>
+  <si>
+    <t>plotOTARResults</t>
   </si>
 </sst>
 </file>
@@ -571,7 +577,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,6 +1177,15 @@
       <c r="A37">
         <v>36</v>
       </c>
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="5">
+        <v>43546</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">

</xml_diff>

<commit_message>
broadcastGenerator is now set by the loaded broadcast algorithm and not config.m
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4083A6-089D-4EB8-962F-D0D6DB60E178}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEBD81A-AB93-40DF-AA75-D1E215BD1022}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="60">
   <si>
     <t>Issue #</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>plotOTARResults</t>
+  </si>
+  <si>
+    <t>update readme.md</t>
   </si>
 </sst>
 </file>
@@ -577,7 +580,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,33 +736,35 @@
         <v>43544</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="5">
-        <v>43542</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="D9" s="6">
+        <v>43542</v>
+      </c>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="5">
-        <v>43542</v>
-      </c>
+      <c r="D10" s="6">
+        <v>43542</v>
+      </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -775,18 +780,21 @@
         <v>43542</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="5">
-        <v>43542</v>
+      <c r="D12" s="7">
+        <v>43542</v>
+      </c>
+      <c r="E12" s="7">
+        <v>43547</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1069,7 +1077,9 @@
       <c r="D29" s="6">
         <v>43545</v>
       </c>
-      <c r="E29" s="6"/>
+      <c r="E29" s="6">
+        <v>43547</v>
+      </c>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -1117,7 +1127,7 @@
         <v>43545</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1131,49 +1141,58 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="34" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="6">
         <v>43546</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="E34" s="6">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="7">
         <v>43546</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="E35" s="7">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="7">
         <v>43546</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="7">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1187,57 +1206,63 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="5">
+        <v>43547</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Added Hameed-Split Algorithm to the list of possible broadcast algorithms
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEBD81A-AB93-40DF-AA75-D1E215BD1022}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7A7099-C541-42D0-B7C0-0F1B0F2F2595}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
   <si>
     <t>Issue #</t>
   </si>
@@ -200,6 +200,21 @@
   </si>
   <si>
     <t>update readme.md</t>
+  </si>
+  <si>
+    <t>Generalize Semi-Rigid to make multiple timout limits</t>
+  </si>
+  <si>
+    <t>generateHameedSemiRigidBroadcast</t>
+  </si>
+  <si>
+    <t>Make normalizeWeights not an internal function</t>
+  </si>
+  <si>
+    <t>generateWeightingSchemeFile</t>
+  </si>
+  <si>
+    <t>Loop through multiple weightingSchemeFiles</t>
   </si>
 </sst>
 </file>
@@ -282,7 +297,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -292,7 +307,6 @@
     <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -580,13 +594,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="86.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1081,20 +1095,22 @@
         <v>43547</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="7">
         <v>43545</v>
       </c>
-      <c r="E30" s="9"/>
+      <c r="E30" s="7">
+        <v>43548</v>
+      </c>
     </row>
     <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -1221,15 +1237,42 @@
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" s="5">
+        <v>43548</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="5">
+        <v>43548</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="5">
+        <v>43548</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added development to master
</commit_message>
<xml_diff>
--- a/IssueTracking.xlsx
+++ b/IssueTracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEBD81A-AB93-40DF-AA75-D1E215BD1022}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7A7099-C541-42D0-B7C0-0F1B0F2F2595}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
   <si>
     <t>Issue #</t>
   </si>
@@ -200,6 +200,21 @@
   </si>
   <si>
     <t>update readme.md</t>
+  </si>
+  <si>
+    <t>Generalize Semi-Rigid to make multiple timout limits</t>
+  </si>
+  <si>
+    <t>generateHameedSemiRigidBroadcast</t>
+  </si>
+  <si>
+    <t>Make normalizeWeights not an internal function</t>
+  </si>
+  <si>
+    <t>generateWeightingSchemeFile</t>
+  </si>
+  <si>
+    <t>Loop through multiple weightingSchemeFiles</t>
   </si>
 </sst>
 </file>
@@ -282,7 +297,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -292,7 +307,6 @@
     <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -580,13 +594,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="86.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1081,20 +1095,22 @@
         <v>43547</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="7">
         <v>43545</v>
       </c>
-      <c r="E30" s="9"/>
+      <c r="E30" s="7">
+        <v>43548</v>
+      </c>
     </row>
     <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -1221,15 +1237,42 @@
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" s="5">
+        <v>43548</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="5">
+        <v>43548</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="5">
+        <v>43548</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>